<commit_message>
Various edits based on a full pass.
</commit_message>
<xml_diff>
--- a/figs_src/data_all_hpca-arial.xlsx
+++ b/figs_src/data_all_hpca-arial.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="7905" yWindow="-15" windowWidth="7980" windowHeight="8970" firstSheet="16" activeTab="18"/>
+    <workbookView xWindow="7905" yWindow="-15" windowWidth="7980" windowHeight="8970" firstSheet="2" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="full_mon" sheetId="4" r:id="rId1"/>
@@ -1407,11 +1407,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="154080768"/>
-        <c:axId val="154082304"/>
+        <c:axId val="154084480"/>
+        <c:axId val="154086016"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="154080768"/>
+        <c:axId val="154084480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1420,7 +1420,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="154082304"/>
+        <c:crossAx val="154086016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1428,7 +1428,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="154082304"/>
+        <c:axId val="154086016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -1452,14 +1452,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="154080768"/>
+        <c:crossAx val="154084480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1732,11 +1731,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="154132864"/>
-        <c:axId val="154134400"/>
+        <c:axId val="154132480"/>
+        <c:axId val="154134016"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="154132864"/>
+        <c:axId val="154132480"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1745,7 +1744,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="low"/>
-        <c:crossAx val="154134400"/>
+        <c:crossAx val="154134016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1753,7 +1752,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="154134400"/>
+        <c:axId val="154134016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="0.60000000000000009"/>
@@ -1785,7 +1784,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="154132864"/>
+        <c:crossAx val="154132480"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2061,11 +2060,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="158561024"/>
-        <c:axId val="158562560"/>
+        <c:axId val="154362240"/>
+        <c:axId val="154363776"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="158561024"/>
+        <c:axId val="154362240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2074,7 +2073,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="158562560"/>
+        <c:crossAx val="154363776"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2082,7 +2081,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="158562560"/>
+        <c:axId val="154363776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2106,14 +2105,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="158561024"/>
+        <c:crossAx val="154362240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2386,11 +2384,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="152124800"/>
-        <c:axId val="152155264"/>
+        <c:axId val="153172992"/>
+        <c:axId val="153203456"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="152124800"/>
+        <c:axId val="153172992"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2399,7 +2397,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="low"/>
-        <c:crossAx val="152155264"/>
+        <c:crossAx val="153203456"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2407,7 +2405,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="152155264"/>
+        <c:axId val="153203456"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2430,14 +2428,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0%" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="152124800"/>
+        <c:crossAx val="153172992"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2876,11 +2873,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="158730496"/>
-        <c:axId val="158752768"/>
+        <c:axId val="154539904"/>
+        <c:axId val="154541440"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="158730496"/>
+        <c:axId val="154539904"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2889,7 +2886,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="158752768"/>
+        <c:crossAx val="154541440"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2897,7 +2894,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="158752768"/>
+        <c:axId val="154541440"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -2927,7 +2924,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="158730496"/>
+        <c:crossAx val="154539904"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -3641,11 +3638,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="151949312"/>
-        <c:axId val="151950848"/>
+        <c:axId val="152997888"/>
+        <c:axId val="152999424"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="151949312"/>
+        <c:axId val="152997888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3654,7 +3651,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="151950848"/>
+        <c:crossAx val="152999424"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3662,7 +3659,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="151950848"/>
+        <c:axId val="152999424"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3700,7 +3697,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="151949312"/>
+        <c:crossAx val="152997888"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -4374,11 +4371,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="151988096"/>
-        <c:axId val="151989632"/>
+        <c:axId val="153036672"/>
+        <c:axId val="153038208"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="151988096"/>
+        <c:axId val="153036672"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4398,7 +4395,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="151989632"/>
+        <c:crossAx val="153038208"/>
         <c:crosses val="autoZero"/>
         <c:auto val="0"/>
         <c:lblAlgn val="ctr"/>
@@ -4406,7 +4403,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="151989632"/>
+        <c:axId val="153038208"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -4444,7 +4441,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="151988096"/>
+        <c:crossAx val="153036672"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5119,11 +5116,11 @@
         </c:dLbls>
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
-        <c:axId val="152182784"/>
-        <c:axId val="152184320"/>
+        <c:axId val="153231360"/>
+        <c:axId val="153232896"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="152182784"/>
+        <c:axId val="153231360"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5132,7 +5129,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="152184320"/>
+        <c:crossAx val="153232896"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5140,7 +5137,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="152184320"/>
+        <c:axId val="153232896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -5164,13 +5161,14 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0%" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="152182784"/>
+        <c:crossAx val="153231360"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -5844,11 +5842,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="152266624"/>
-        <c:axId val="152268160"/>
+        <c:axId val="153316736"/>
+        <c:axId val="153322624"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="152266624"/>
+        <c:axId val="153316736"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5868,7 +5866,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="152268160"/>
+        <c:crossAx val="153322624"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -5876,7 +5874,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="152268160"/>
+        <c:axId val="153322624"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -5906,7 +5904,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="152266624"/>
+        <c:crossAx val="153316736"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -6582,7 +6580,7 @@
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
         <c:axId val="153423232"/>
-        <c:axId val="153425024"/>
+        <c:axId val="153429120"/>
       </c:barChart>
       <c:catAx>
         <c:axId val="153423232"/>
@@ -6594,7 +6592,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="153425024"/>
+        <c:crossAx val="153429120"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -6602,7 +6600,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="153425024"/>
+        <c:axId val="153429120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -7457,7 +7455,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0%" sourceLinked="1"/>
@@ -7938,11 +7935,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:gapWidth val="150"/>
-        <c:axId val="153681280"/>
-        <c:axId val="153760896"/>
+        <c:axId val="153750912"/>
+        <c:axId val="153769088"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="153681280"/>
+        <c:axId val="153750912"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7962,7 +7959,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="153760896"/>
+        <c:crossAx val="153769088"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -7970,7 +7967,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="153760896"/>
+        <c:axId val="153769088"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -7993,14 +7990,13 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0%" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="153681280"/>
+        <c:crossAx val="153750912"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -8776,7 +8772,7 @@
         <c:gapWidth val="150"/>
         <c:overlap val="100"/>
         <c:axId val="153848064"/>
-        <c:axId val="153862144"/>
+        <c:axId val="153866240"/>
       </c:barChart>
       <c:catAx>
         <c:axId val="153848064"/>
@@ -8788,7 +8784,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="153862144"/>
+        <c:crossAx val="153866240"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -8796,7 +8792,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="153862144"/>
+        <c:axId val="153866240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="1"/>
@@ -8820,7 +8816,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0%" sourceLinked="1"/>
@@ -8899,7 +8894,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="260" workbookViewId="0" zoomToFit="1"/>
+    <sheetView zoomScale="260" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="156" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -8971,7 +8966,7 @@
 <chartsheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <sheetPr/>
   <sheetViews>
-    <sheetView zoomScale="243" workbookViewId="0" zoomToFit="1"/>
+    <sheetView tabSelected="1" zoomScale="260" workbookViewId="0" zoomToFit="1"/>
   </sheetViews>
   <pageMargins left="0" right="0" top="0" bottom="0" header="0" footer="0"/>
   <pageSetup paperSize="156" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
@@ -9518,7 +9513,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="3080926" cy="2179383"/>
+    <xdr:ext cx="2927106" cy="2025894"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1"/>

</xml_diff>